<commit_message>
refactor code change function export excel
</commit_message>
<xml_diff>
--- a/testdata/test.xlsx
+++ b/testdata/test.xlsx
@@ -26,24 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>RoleCode</t>
-  </si>
-  <si>
-    <t>RoleType</t>
-  </si>
-  <si>
-    <t>user1</t>
-  </si>
-  <si>
     <t>pass1</t>
   </si>
   <si>
@@ -53,20 +35,38 @@
     <t>ADMIN</t>
   </si>
   <si>
-    <t>user4</t>
-  </si>
-  <si>
-    <t>sample4@gmail.com</t>
-  </si>
-  <si>
     <t>test123@gmail.com</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>rolecode</t>
+  </si>
+  <si>
+    <t>roletype</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>testcheck@gmail.com</t>
+  </si>
+  <si>
+    <t>user12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +78,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,9 +112,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -391,7 +400,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -404,64 +413,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C3" s="1"/>
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
+      <c r="C4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add full error messages
</commit_message>
<xml_diff>
--- a/testdata/test.xlsx
+++ b/testdata/test.xlsx
@@ -24,20 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>pass1</t>
   </si>
   <si>
-    <t>USER</t>
-  </si>
-  <si>
-    <t>ADMIN</t>
-  </si>
-  <si>
-    <t>test123@gmail.com</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -53,13 +44,10 @@
     <t>username</t>
   </si>
   <si>
-    <t>user2</t>
-  </si>
-  <si>
-    <t>testcheck@gmail.com</t>
-  </si>
-  <si>
-    <t>user12</t>
+    <t>123@gmail.coms</t>
+  </si>
+  <si>
+    <t>MANAGER</t>
   </si>
 </sst>
 </file>
@@ -400,7 +388,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,54 +402,40 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
+      <c r="A2">
+        <v>123</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
@@ -469,9 +443,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>